<commit_message>
bug fixes / new data
</commit_message>
<xml_diff>
--- a/NTDS_Template.xlsx
+++ b/NTDS_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9000" windowWidth="28800" windowHeight="12195"/>
+    <workbookView xWindow="0" yWindow="10800" windowWidth="28800" windowHeight="12195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Nummer</t>
   </si>
   <si>
-    <t>Naam</t>
-  </si>
-  <si>
     <t>E-mail</t>
   </si>
   <si>
@@ -47,12 +44,6 @@
     <t>Partner Latin</t>
   </si>
   <si>
-    <t>Ballroom lead/follow</t>
-  </si>
-  <si>
-    <t>Latin lead/follow</t>
-  </si>
-  <si>
     <t>Ballroom verplicht blind daten</t>
   </si>
   <si>
@@ -68,21 +59,12 @@
     <t>Slaapplek</t>
   </si>
   <si>
-    <t>Wil jureren</t>
-  </si>
-  <si>
     <t>Ja/Null</t>
   </si>
   <si>
-    <t>NTDS/Zelf</t>
-  </si>
-  <si>
     <t>Lead/Follow</t>
   </si>
   <si>
-    <t>Beginner/Breiten/Open</t>
-  </si>
-  <si>
     <t>TEXT</t>
   </si>
   <si>
@@ -99,6 +81,45 @@
   </si>
   <si>
     <t>EHBO</t>
+  </si>
+  <si>
+    <t>Beginner/Breiten/Open/Null</t>
+  </si>
+  <si>
+    <t>BHV</t>
+  </si>
+  <si>
+    <t>Ja/Misschien/Null</t>
+  </si>
+  <si>
+    <t>Voornaam</t>
+  </si>
+  <si>
+    <t>Tussenvoegsel</t>
+  </si>
+  <si>
+    <t>Achternaam</t>
+  </si>
+  <si>
+    <t>Ballroom rol</t>
+  </si>
+  <si>
+    <t>Latin rol</t>
+  </si>
+  <si>
+    <t>Jury ballroom</t>
+  </si>
+  <si>
+    <t>Jury latin</t>
+  </si>
+  <si>
+    <t>Nu vrijwilliger</t>
+  </si>
+  <si>
+    <t>Eerder vrijwilliger geweest</t>
+  </si>
+  <si>
+    <t>NTDS/Null</t>
   </si>
 </sst>
 </file>
@@ -454,99 +475,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="11" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" customWidth="1"/>
-    <col min="15" max="15" width="8" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" customWidth="1"/>
+    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
       </c>
       <c r="H3" t="s">
         <v>17</v>
@@ -555,28 +604,46 @@
         <v>17</v>
       </c>
       <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="T3" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V3" t="s">
         <v>21</v>
       </c>
-      <c r="P3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>19</v>
+      <c r="W3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>